<commit_message>
add bgez blez sltu sltiu sra lb lh lbu lhu sb sh modify bus and related component doesn't test we signal is now [3:0]we
</commit_message>
<xml_diff>
--- a/doc/指令.xlsx
+++ b/doc/指令.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="116">
   <si>
     <t>add</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -399,6 +399,86 @@
   </si>
   <si>
     <t>发生异常以及eret的优先级比stall高，如果此时有stall会强行写入pc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sra</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>算术</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sltu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>算术</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sltiu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>算术</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blez</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bgtz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lbu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lhu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -756,10 +836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T65"/>
+  <dimension ref="A1:T76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1078,30 +1158,30 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="H13">
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="J13" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
         <v>47</v>
@@ -1124,30 +1204,30 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="J15" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
         <v>47</v>
@@ -1168,35 +1248,35 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>96</v>
       </c>
       <c r="B17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>98</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>99</v>
+      </c>
+      <c r="J17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
         <v>47</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="I17" t="s">
-        <v>58</v>
-      </c>
-      <c r="J17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" t="s">
-        <v>42</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1214,12 +1294,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1237,12 +1317,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1260,9 +1340,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
         <v>42</v>
@@ -1283,9 +1363,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
         <v>42</v>
@@ -1306,9 +1386,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
         <v>42</v>
@@ -1329,9 +1409,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
         <v>42</v>
@@ -1352,94 +1432,88 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>58</v>
+      </c>
+      <c r="J25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26" t="s">
+        <v>58</v>
+      </c>
+      <c r="J26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>66</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27" t="s">
+        <v>58</v>
+      </c>
+      <c r="J27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
         <v>12</v>
-      </c>
-      <c r="B25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>66</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-      <c r="L25" t="s">
-        <v>66</v>
-      </c>
-      <c r="M25" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>66</v>
-      </c>
-      <c r="H26">
-        <v>1</v>
-      </c>
-      <c r="I26" t="s">
-        <v>76</v>
-      </c>
-      <c r="J26" t="s">
-        <v>62</v>
-      </c>
-      <c r="K26">
-        <v>1</v>
-      </c>
-      <c r="L26" t="s">
-        <v>66</v>
-      </c>
-      <c r="M26" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A27" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" t="s">
-        <v>43</v>
-      </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-      <c r="I27" t="s">
-        <v>76</v>
-      </c>
-      <c r="J27" t="s">
-        <v>62</v>
-      </c>
-      <c r="K27">
-        <v>1</v>
-      </c>
-      <c r="L27" t="s">
-        <v>66</v>
-      </c>
-      <c r="M27" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A28" t="s">
-        <v>9</v>
       </c>
       <c r="B28" t="s">
         <v>43</v>
       </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>66</v>
+      </c>
       <c r="K28">
         <v>1</v>
       </c>
@@ -1450,9 +1524,9 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B29" t="s">
         <v>43</v>
@@ -1463,6 +1537,15 @@
       <c r="D29" t="s">
         <v>66</v>
       </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J29" t="s">
+        <v>62</v>
+      </c>
       <c r="K29">
         <v>1</v>
       </c>
@@ -1473,18 +1556,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
         <v>43</v>
       </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>67</v>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30" t="s">
+        <v>76</v>
+      </c>
+      <c r="J30" t="s">
+        <v>62</v>
       </c>
       <c r="K30">
         <v>1</v>
@@ -1496,52 +1582,52 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
-        <v>67</v>
-      </c>
-      <c r="R31">
-        <v>1</v>
-      </c>
-      <c r="S31" t="s">
-        <v>66</v>
-      </c>
-      <c r="T31" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.15">
+        <v>43</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31" t="s">
+        <v>66</v>
+      </c>
+      <c r="M31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
-      </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
-      <c r="I32" t="s">
-        <v>59</v>
-      </c>
-      <c r="J32" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
+        <v>43</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>66</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32" t="s">
+        <v>66</v>
+      </c>
+      <c r="M32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -1549,77 +1635,68 @@
       <c r="D33" t="s">
         <v>67</v>
       </c>
-      <c r="N33">
-        <v>1</v>
-      </c>
-      <c r="O33" t="s">
-        <v>70</v>
-      </c>
-      <c r="P33" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33" t="s">
+        <v>66</v>
+      </c>
+      <c r="M33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>108</v>
       </c>
       <c r="B34" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>67</v>
-      </c>
-      <c r="N34">
-        <v>1</v>
-      </c>
-      <c r="O34" t="s">
-        <v>70</v>
-      </c>
-      <c r="P34" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
+        <v>65</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34" t="s">
+        <v>103</v>
+      </c>
+      <c r="M34" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>109</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>67</v>
-      </c>
-      <c r="H35">
-        <v>1</v>
-      </c>
-      <c r="I35" t="s">
-        <v>59</v>
-      </c>
-      <c r="J35" t="s">
-        <v>61</v>
-      </c>
-      <c r="N35">
-        <v>1</v>
-      </c>
-      <c r="O35" t="s">
-        <v>70</v>
-      </c>
-      <c r="P35" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
+        <v>65</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35" t="s">
+        <v>103</v>
+      </c>
+      <c r="M35" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1627,320 +1704,552 @@
       <c r="D36" t="s">
         <v>67</v>
       </c>
-      <c r="N36">
-        <v>1</v>
-      </c>
-      <c r="O36" t="s">
+      <c r="R36">
+        <v>1</v>
+      </c>
+      <c r="S36" t="s">
+        <v>66</v>
+      </c>
+      <c r="T36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
         <v>65</v>
       </c>
-      <c r="P36" t="s">
+      <c r="R37">
+        <v>1</v>
+      </c>
+      <c r="S37" t="s">
+        <v>65</v>
+      </c>
+      <c r="T37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>65</v>
+      </c>
+      <c r="R38">
+        <v>1</v>
+      </c>
+      <c r="S38" t="s">
+        <v>65</v>
+      </c>
+      <c r="T38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>45</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39" t="s">
+        <v>59</v>
+      </c>
+      <c r="J39" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40" t="s">
+        <v>57</v>
+      </c>
+      <c r="J40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" t="s">
+        <v>45</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41" t="s">
+        <v>57</v>
+      </c>
+      <c r="J41" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42" t="s">
+        <v>45</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>57</v>
+      </c>
+      <c r="J42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43" t="s">
+        <v>57</v>
+      </c>
+      <c r="J43" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>67</v>
+      </c>
+      <c r="N44">
+        <v>1</v>
+      </c>
+      <c r="O44" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A37" t="s">
+      <c r="P44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>67</v>
+      </c>
+      <c r="N45">
+        <v>1</v>
+      </c>
+      <c r="O45" t="s">
+        <v>70</v>
+      </c>
+      <c r="P45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46" t="s">
+        <v>59</v>
+      </c>
+      <c r="J46" t="s">
+        <v>61</v>
+      </c>
+      <c r="N46">
+        <v>1</v>
+      </c>
+      <c r="O46" t="s">
+        <v>70</v>
+      </c>
+      <c r="P46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>67</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
+      <c r="O47" t="s">
+        <v>65</v>
+      </c>
+      <c r="P47" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
         <v>23</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B48" t="s">
         <v>46</v>
       </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
         <v>67</v>
       </c>
-      <c r="N37">
-        <v>1</v>
-      </c>
-      <c r="O37" t="s">
+      <c r="N48">
+        <v>1</v>
+      </c>
+      <c r="O48" t="s">
         <v>67</v>
       </c>
-      <c r="P37" t="s">
+      <c r="P48" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A38" t="s">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
         <v>21</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B49" t="s">
         <v>46</v>
       </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
         <v>67</v>
       </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" t="s">
         <v>81</v>
       </c>
-      <c r="N38">
-        <v>1</v>
-      </c>
-      <c r="O38" t="s">
+      <c r="N49">
+        <v>1</v>
+      </c>
+      <c r="O49" t="s">
         <v>71</v>
       </c>
-      <c r="P38" t="s">
+      <c r="P49" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A39" t="s">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
         <v>20</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B50" t="s">
         <v>46</v>
       </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
         <v>67</v>
       </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" t="s">
         <v>71</v>
       </c>
-      <c r="N39">
-        <v>1</v>
-      </c>
-      <c r="O39" t="s">
+      <c r="N50">
+        <v>1</v>
+      </c>
+      <c r="O50" t="s">
         <v>71</v>
       </c>
-      <c r="P39" t="s">
+      <c r="P50" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A40" t="s">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A51" t="s">
         <v>19</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B51" t="s">
         <v>46</v>
       </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-      <c r="F40" t="s">
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" t="s">
         <v>71</v>
       </c>
-      <c r="H40">
-        <v>1</v>
-      </c>
-      <c r="I40" t="s">
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51" t="s">
         <v>59</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J51" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A41" t="s">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A52" t="s">
         <v>18</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B52" t="s">
         <v>46</v>
       </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-      <c r="F41" t="s">
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
         <v>71</v>
       </c>
-      <c r="H41">
-        <v>1</v>
-      </c>
-      <c r="I41" t="s">
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52" t="s">
         <v>59</v>
       </c>
-      <c r="J41" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A42" t="s">
+      <c r="J52" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A53" t="s">
         <v>16</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B53" t="s">
         <v>46</v>
       </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
         <v>67</v>
       </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" t="s">
         <v>71</v>
       </c>
-      <c r="N42">
-        <v>1</v>
-      </c>
-      <c r="O42" t="s">
+      <c r="N53">
+        <v>1</v>
+      </c>
+      <c r="O53" t="s">
         <v>71</v>
       </c>
-      <c r="P42" t="s">
+      <c r="P53" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A43" t="s">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A54" t="s">
         <v>15</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B54" t="s">
         <v>46</v>
       </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
         <v>67</v>
       </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" t="s">
         <v>71</v>
       </c>
-      <c r="N43">
-        <v>1</v>
-      </c>
-      <c r="O43" t="s">
+      <c r="N54">
+        <v>1</v>
+      </c>
+      <c r="O54" t="s">
         <v>71</v>
       </c>
-      <c r="P43" t="s">
+      <c r="P54" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A52" s="2" t="s">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A63" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A53" s="2" t="s">
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A64" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
-      <c r="M53" s="2"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A54" s="2" t="s">
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+      <c r="M64" s="2"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A65" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
-      <c r="L54" s="2"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1" t="s">
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
-      <c r="L55" s="1"/>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A56" t="s">
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A67" t="s">
         <v>88</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B67" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A57" t="s">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A68" t="s">
         <v>84</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B68" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A58" t="s">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A69" t="s">
         <v>85</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B69" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A59" t="s">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A70" t="s">
         <v>86</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B70" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A61" t="s">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A72" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A62" t="s">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A73" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A63" t="s">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A74" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A64" t="s">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A75" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A65" t="s">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A76" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1949,9 +2258,9 @@
     <sortCondition descending="1" ref="B2:B42"/>
   </sortState>
   <mergeCells count="3">
-    <mergeCell ref="A52:L52"/>
-    <mergeCell ref="A53:M53"/>
-    <mergeCell ref="A54:L54"/>
+    <mergeCell ref="A63:L63"/>
+    <mergeCell ref="A64:M64"/>
+    <mergeCell ref="A65:L65"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>